<commit_message>
Updates BoM with exact components used
</commit_message>
<xml_diff>
--- a/ExpBoard_BoM.xlsx
+++ b/ExpBoard_BoM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Bill of materials</t>
   </si>
@@ -108,12 +108,6 @@
     <t>0.1" Pin header</t>
   </si>
   <si>
-    <t>RE04698??</t>
-  </si>
-  <si>
-    <t>CN14493??</t>
-  </si>
-  <si>
     <t>CPC</t>
   </si>
   <si>
@@ -123,30 +117,6 @@
     <t>eBay</t>
   </si>
   <si>
-    <t>LS03781??</t>
-  </si>
-  <si>
-    <t>Price exVAT (£)</t>
-  </si>
-  <si>
-    <t>9411887???</t>
-  </si>
-  <si>
-    <t>1960939??</t>
-  </si>
-  <si>
-    <t>RE06540??</t>
-  </si>
-  <si>
-    <t>Quantity required</t>
-  </si>
-  <si>
-    <t>Total cost (ex VAT)</t>
-  </si>
-  <si>
-    <t>Total per board</t>
-  </si>
-  <si>
     <t>1438760</t>
   </si>
   <si>
@@ -154,23 +124,103 @@
   </si>
   <si>
     <t>TRI-LED</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>Blue 5mm LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1855507 </t>
+  </si>
+  <si>
+    <t>10K 0.25W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9339060 </t>
+  </si>
+  <si>
+    <t>100R 0.25W</t>
+  </si>
+  <si>
+    <t>9339043</t>
+  </si>
+  <si>
+    <t>150R 0.25W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9339175 </t>
+  </si>
+  <si>
+    <t>LS03781</t>
+  </si>
+  <si>
+    <t>RE04698</t>
+  </si>
+  <si>
+    <t>CN14535</t>
+  </si>
+  <si>
+    <t>0.1UF, 50V, Y5V</t>
+  </si>
+  <si>
+    <t>9411887</t>
+  </si>
+  <si>
+    <t>TMP36GT9Z</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>9608230</t>
+  </si>
+  <si>
+    <t>10way, 1 row, Socket</t>
+  </si>
+  <si>
+    <t>Tactile</t>
+  </si>
+  <si>
+    <t>1960939</t>
+  </si>
+  <si>
+    <t>Green 5mm LED</t>
+  </si>
+  <si>
+    <t>1461633</t>
+  </si>
+  <si>
+    <t>Red LED 5mm</t>
+  </si>
+  <si>
+    <t>1461624</t>
+  </si>
+  <si>
+    <t>T1 3/4, 20mA, 2V</t>
+  </si>
+  <si>
+    <t>5V, 1mA</t>
+  </si>
+  <si>
+    <t>T1 3/4, 20mA, 3.2V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,9 +246,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -501,26 +550,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -536,219 +585,268 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="F5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="F8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>35</v>
-      </c>
-      <c r="F11">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
       <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
       <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19">
-        <f>SUM(F4:F17)</f>
-        <v>3.0700000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F21">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23">
-        <f>F19*F21</f>
-        <v>107.45000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>